<commit_message>
small change to file-reader
</commit_message>
<xml_diff>
--- a/digipalvelut-projekti/static/test.xlsx
+++ b/digipalvelut-projekti/static/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\digipalvelut-projekti\digipalvelut-projekti\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CC0B980-155D-486E-8D42-4D38CA22E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590DE7F-C778-4FAD-8908-665F7E9754C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
+    <workbookView xWindow="-23640" yWindow="2355" windowWidth="14400" windowHeight="7275" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,31 +36,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
+    <t>Participated students</t>
+  </si>
+  <si>
+    <t>Helpfullness of the environment</t>
+  </si>
+  <si>
+    <t>Unit of the value</t>
+  </si>
+  <si>
+    <t>Number of persons</t>
+  </si>
+  <si>
+    <t>Value from the questionnaires</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF104861"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,8 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -422,44 +464,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF3E864-219C-432C-85A8-BAC3BB0B0A64}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>80</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+      <c r="B3" s="2">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="2">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -690,20 +768,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,14 +804,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB3B2CB-9EE9-4AC4-9E93-74508007D977}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -748,4 +818,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
copied the values from example file
</commit_message>
<xml_diff>
--- a/digipalvelut-projekti/static/test.xlsx
+++ b/digipalvelut-projekti/static/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\digipalvelut-projekti\digipalvelut-projekti\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590DE7F-C778-4FAD-8908-665F7E9754C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEE47F-9964-435A-A627-4E19699C2981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23640" yWindow="2355" windowWidth="14400" windowHeight="7275" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>Helpfullness of the environment</t>
   </si>
   <si>
-    <t>Unit of the value</t>
-  </si>
-  <si>
     <t>Number of persons</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,19 +485,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="3"/>
     </row>
@@ -518,7 +518,7 @@
         <v>1.6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -538,7 +538,7 @@
         <v>0.75</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -768,20 +768,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,6 +804,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB3B2CB-9EE9-4AC4-9E93-74508007D977}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -818,12 +826,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
font added to global-styles
</commit_message>
<xml_diff>
--- a/digipalvelut-projekti/static/test.xlsx
+++ b/digipalvelut-projekti/static/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\digipalvelut-projekti\digipalvelut-projekti\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEE47F-9964-435A-A627-4E19699C2981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7C952C-D2B6-404A-BCA9-9C942319E208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23640" yWindow="2355" windowWidth="14400" windowHeight="7275" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Participated students</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,28 +482,28 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>
@@ -518,12 +518,12 @@
         <v>1.6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>80</v>
@@ -538,7 +538,7 @@
         <v>0.75</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -768,20 +768,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,14 +804,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB3B2CB-9EE9-4AC4-9E93-74508007D977}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -826,4 +818,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
end, target variables renamed everywhere
</commit_message>
<xml_diff>
--- a/digipalvelut-projekti/static/test.xlsx
+++ b/digipalvelut-projekti/static/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gr289361\Desktop\projekti\digipalvelut-projekti\digipalvelut-projekti\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93165B0A-83AF-4B93-984F-2ACFE922AE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209745B-47F9-401A-B49C-166A185BC2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1010" windowWidth="14400" windowHeight="7280" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D048ECE2-60FA-4AD2-9F24-90A95A17B271}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
   </si>
   <si>
     <t>Unit</t>
@@ -63,6 +57,12 @@
   </si>
   <si>
     <t>Value from the questionnaires</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,25 +478,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>
@@ -508,12 +508,12 @@
         <v>80</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>80</v>
@@ -525,7 +525,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -755,20 +755,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e3c136e-bc0f-422c-9118-1fc0803c8724" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -791,6 +791,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB3B2CB-9EE9-4AC4-9E93-74508007D977}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -805,12 +813,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC32B3D8-B429-49D9-AF05-52347C931EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>